<commit_message>
Removed timer in validlogingtest and invalidlogintest so that test cases can run faster. Set a timer for the shoppingcarttest so that each of the action can be viewed for the purpose of this code challenge
</commit_message>
<xml_diff>
--- a/TestData/InValidLoginCredentials.xlsx
+++ b/TestData/InValidLoginCredentials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationChallengeCode\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C33DC72-7B49-406E-805E-D1F1C0582BD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7EBFFF-CE71-4099-A09B-92BDD1BD2720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2810" yWindow="1520" windowWidth="14400" windowHeight="8140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="2540" windowWidth="14400" windowHeight="8140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>